<commit_message>
main : Sources updated
</commit_message>
<xml_diff>
--- a/report/assets/InformationalModel/InformationalModelTypes.xlsx
+++ b/report/assets/InformationalModel/InformationalModelTypes.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="74">
   <si>
     <t xml:space="preserve">Таблица - Словарь данных таблицы DE_DOC_OrderCreationInventoryCommission</t>
   </si>
@@ -74,7 +74,7 @@
     <t xml:space="preserve">DE_CTL_MyOrganizations</t>
   </si>
   <si>
-    <t xml:space="preserve">de_storageLocationId</t>
+    <t xml:space="preserve">de_storageLocationsId</t>
   </si>
   <si>
     <t xml:space="preserve">Место хранения</t>
@@ -134,10 +134,10 @@
     <t xml:space="preserve">de_positionsId</t>
   </si>
   <si>
-    <t xml:space="preserve">Должность</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DE_CTL_Positions</t>
+    <t xml:space="preserve">Должность сотрудника</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DE_CTL_EmployeePosition</t>
   </si>
   <si>
     <t xml:space="preserve">Таблица - Словарь данных таблицы DE_TAB_ListInventoryCommission</t>
@@ -149,7 +149,7 @@
     <t xml:space="preserve">DE_DOC_OrderCreationInventoryCommission</t>
   </si>
   <si>
-    <t xml:space="preserve">de_employeeId</t>
+    <t xml:space="preserve">de_employeesId</t>
   </si>
   <si>
     <t xml:space="preserve">Код сотрудника</t>
@@ -173,7 +173,43 @@
     <t xml:space="preserve">DE_DOC_InventoryList</t>
   </si>
   <si>
+    <t xml:space="preserve">de_nomenclaturesId</t>
+  </si>
+  <si>
     <t xml:space="preserve">Код номенклатуры</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DE_CTL_Nomenclatures</t>
+  </si>
+  <si>
+    <t xml:space="preserve">de_cost</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Цена</t>
+  </si>
+  <si>
+    <t xml:space="preserve">de_accountingQuantity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Кол-во по данным бух. учета</t>
+  </si>
+  <si>
+    <t xml:space="preserve">de_actualQuantity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Кол-во фактическое</t>
+  </si>
+  <si>
+    <t xml:space="preserve">de_shortageQuantity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Кол-во недостачи</t>
+  </si>
+  <si>
+    <t xml:space="preserve">de_surplusQuantity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Кол-во излишков</t>
   </si>
   <si>
     <t xml:space="preserve">Таблица - Словарь данных таблицы DE_CTL_Nomenclatures</t>
@@ -346,18 +382,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D1004"/>
+  <dimension ref="A1:D1009"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D28" activeCellId="0" sqref="A22:D28"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A43" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D56" activeCellId="0" sqref="A47:D56"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.640625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.25"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="26.05"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="36.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="23.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="36.3"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -950,52 +986,66 @@
     </row>
     <row r="51" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="5" t="s">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="B51" s="5" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C51" s="5" t="s">
         <v>15</v>
       </c>
       <c r="D51" s="5" t="s">
-        <v>44</v>
+        <v>52</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="1"/>
-      <c r="B52" s="1"/>
-      <c r="C52" s="1"/>
-      <c r="D52" s="1"/>
+      <c r="A52" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B52" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C52" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D52" s="5" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="53" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="B53" s="2"/>
-      <c r="C53" s="2"/>
-      <c r="D53" s="2"/>
-    </row>
-    <row r="54" customFormat="false" ht="23.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A54" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B54" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C54" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D54" s="3" t="s">
-        <v>4</v>
+      <c r="A53" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="B53" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C53" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D53" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="B54" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="C54" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D54" s="5" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="5" t="s">
-        <v>5</v>
+        <v>59</v>
       </c>
       <c r="B55" s="5" t="s">
-        <v>26</v>
+        <v>60</v>
       </c>
       <c r="C55" s="5" t="s">
         <v>15</v>
@@ -1006,114 +1056,114 @@
     </row>
     <row r="56" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="5" t="s">
-        <v>27</v>
+        <v>61</v>
       </c>
       <c r="B56" s="5" t="s">
-        <v>28</v>
+        <v>62</v>
       </c>
       <c r="C56" s="5" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="D56" s="5" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="B57" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="C57" s="5" t="s">
+      <c r="A57" s="1"/>
+      <c r="B57" s="1"/>
+      <c r="C57" s="1"/>
+      <c r="D57" s="1"/>
+    </row>
+    <row r="58" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B58" s="2"/>
+      <c r="C58" s="2"/>
+      <c r="D58" s="2"/>
+    </row>
+    <row r="59" customFormat="false" ht="23.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A59" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B59" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C59" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D59" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B60" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C60" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D60" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B61" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C61" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D57" s="5" t="s">
+      <c r="D61" s="5" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="58" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="B58" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="C58" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="D58" s="5" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="59" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="B59" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="C59" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="D59" s="5" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="60" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="1"/>
-      <c r="B60" s="1"/>
-      <c r="C60" s="1"/>
-      <c r="D60" s="1"/>
-    </row>
-    <row r="61" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="B61" s="2"/>
-      <c r="C61" s="2"/>
-      <c r="D61" s="2"/>
-    </row>
-    <row r="62" customFormat="false" ht="23.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A62" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B62" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C62" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D62" s="3" t="s">
-        <v>4</v>
+    <row r="62" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="B62" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="C62" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D62" s="5" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="5" t="s">
-        <v>5</v>
+        <v>66</v>
       </c>
       <c r="B63" s="5" t="s">
-        <v>26</v>
+        <v>67</v>
       </c>
       <c r="C63" s="5" t="s">
         <v>15</v>
       </c>
       <c r="D63" s="5" t="s">
-        <v>8</v>
+        <v>68</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="5" t="s">
-        <v>27</v>
+        <v>69</v>
       </c>
       <c r="B64" s="5" t="s">
-        <v>28</v>
+        <v>70</v>
       </c>
       <c r="C64" s="5" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="D64" s="5" t="s">
-        <v>8</v>
+        <v>71</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1124,7 +1174,7 @@
     </row>
     <row r="66" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="2" t="s">
-        <v>61</v>
+        <v>72</v>
       </c>
       <c r="B66" s="2"/>
       <c r="C66" s="2"/>
@@ -1179,28 +1229,54 @@
       <c r="D70" s="1"/>
     </row>
     <row r="71" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="1"/>
-      <c r="B71" s="1"/>
-      <c r="C71" s="1"/>
-      <c r="D71" s="1"/>
-    </row>
-    <row r="72" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A72" s="1"/>
-      <c r="B72" s="1"/>
-      <c r="C72" s="1"/>
-      <c r="D72" s="1"/>
+      <c r="A71" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B71" s="2"/>
+      <c r="C71" s="2"/>
+      <c r="D71" s="2"/>
+    </row>
+    <row r="72" customFormat="false" ht="23.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A72" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B72" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C72" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D72" s="3" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="73" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A73" s="1"/>
-      <c r="B73" s="1"/>
-      <c r="C73" s="1"/>
-      <c r="D73" s="1"/>
+      <c r="A73" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B73" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C73" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D73" s="5" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="74" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A74" s="1"/>
-      <c r="B74" s="1"/>
-      <c r="C74" s="1"/>
-      <c r="D74" s="1"/>
+      <c r="A74" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B74" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C74" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D74" s="5" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="75" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="1"/>
@@ -6781,6 +6857,36 @@
       <c r="B1004" s="1"/>
       <c r="C1004" s="1"/>
       <c r="D1004" s="1"/>
+    </row>
+    <row r="1005" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1005" s="1"/>
+      <c r="B1005" s="1"/>
+      <c r="C1005" s="1"/>
+      <c r="D1005" s="1"/>
+    </row>
+    <row r="1006" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1006" s="1"/>
+      <c r="B1006" s="1"/>
+      <c r="C1006" s="1"/>
+      <c r="D1006" s="1"/>
+    </row>
+    <row r="1007" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1007" s="1"/>
+      <c r="B1007" s="1"/>
+      <c r="C1007" s="1"/>
+      <c r="D1007" s="1"/>
+    </row>
+    <row r="1008" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1008" s="1"/>
+      <c r="B1008" s="1"/>
+      <c r="C1008" s="1"/>
+      <c r="D1008" s="1"/>
+    </row>
+    <row r="1009" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1009" s="1"/>
+      <c r="B1009" s="1"/>
+      <c r="C1009" s="1"/>
+      <c r="D1009" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="11">
@@ -6792,9 +6898,9 @@
     <mergeCell ref="A36:D36"/>
     <mergeCell ref="A41:D41"/>
     <mergeCell ref="A47:D47"/>
-    <mergeCell ref="A53:D53"/>
-    <mergeCell ref="A61:D61"/>
+    <mergeCell ref="A58:D58"/>
     <mergeCell ref="A66:D66"/>
+    <mergeCell ref="A71:D71"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>